<commit_message>
DCM and PGM commit on 20230924
</commit_message>
<xml_diff>
--- a/03.設計/詳細設計書_STB01（MAIN）.xlsx
+++ b/03.設計/詳細設計書_STB01（MAIN）.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="129">
   <si>
     <t>プロジェクト番号</t>
     <rPh sb="6" eb="8">
@@ -348,53 +348,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・表示中の画面がプレイ画面の場合、総プレイ時間変数を +1 する</t>
-    <rPh sb="1" eb="4">
-      <t>ヒョウジチュウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ソウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・表示中の画面がマニュアル画面以外の場合、画面表示時間変数を +1 する</t>
-    <rPh sb="13" eb="15">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="23" eb="27">
-      <t>ヒョウジジカン</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>3.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -533,16 +486,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・ゲーム設定を初期化（）</t>
-    <rPh sb="4" eb="6">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="7" eb="10">
-      <t>ショキカ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・プレイ画面に遷移</t>
     <rPh sb="4" eb="6">
       <t>ガメン</t>
@@ -593,19 +536,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・タイトル、キー案内の文言を表示（）</t>
-    <rPh sb="8" eb="10">
-      <t>アンナイ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>モンゴン</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・コース変数を +1 する</t>
     <rPh sb="4" eb="6">
       <t>ヘンスウ</t>
@@ -613,32 +543,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・コースごとのゲーム設定処理を実行（）</t>
-    <rPh sb="10" eb="12">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・入力された方向キーによってプレイヤーを動かす（）</t>
-    <rPh sb="1" eb="3">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ホウコウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ウゴ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・全体スタン中以外の場合、エネミーを動かす（）</t>
     <rPh sb="1" eb="3">
       <t>ゼンタイ</t>
@@ -655,26 +559,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・アイテム使用のチェックを実行する（）</t>
-    <rPh sb="5" eb="7">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・各種オブジェクトのヒットチェックを実行する（）</t>
-    <rPh sb="1" eb="3">
-      <t>カクシュ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・エネミー生成判定を実行する（）</t>
     <rPh sb="5" eb="9">
       <t>セイセイハンテイ</t>
@@ -685,49 +569,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・ゴール生成判定を実行する（）</t>
-    <rPh sb="4" eb="8">
-      <t>セイセイハンテイ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・アイテム生成判定を実行する（）</t>
-    <rPh sb="5" eb="9">
-      <t>セイセイハンテイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・アイテムを使用中の場合、アイテム使用中変数を -1 する</t>
-    <rPh sb="6" eb="9">
-      <t>シヨウチュウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・アイテム使用中変数が 0 の場合、アイテムの効果を無効化する（）</t>
-    <rPh sb="5" eb="8">
-      <t>シヨウチュウ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・プレイヤーが無敵の場合、無敵中変数を -1 する</t>
     <rPh sb="7" eb="9">
       <t>ムテキ</t>
@@ -826,38 +667,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・ゴールした場合、画面表示時間変数を初期化する</t>
-    <rPh sb="6" eb="8">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="9" eb="17">
-      <t>ガメンヒョウジジカンヘンスウ</t>
-    </rPh>
-    <rPh sb="18" eb="21">
-      <t>ショキカ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・画面表示時間変数が 1 の場合、下記処理を実施</t>
-    <rPh sb="1" eb="5">
-      <t>ガメンヒョウジ</t>
-    </rPh>
-    <rPh sb="5" eb="9">
-      <t>ジカンヘンスウ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="17" eb="21">
-      <t>カキショリ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジッシ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>7.</t>
   </si>
   <si>
@@ -871,26 +680,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・キー案内の文言を表示（）</t>
-    <rPh sb="3" eb="5">
-      <t>アンナイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>モンゴン</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・マニュアルを表示</t>
-    <rPh sb="7" eb="9">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・スペースキーを押下でプレイ画面に遷移</t>
     <rPh sb="8" eb="10">
       <t>オウカ</t>
@@ -957,51 +746,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・コースフィールド（迷路）の配列を作成（）</t>
-    <rPh sb="10" eb="12">
-      <t>メイロ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ハイレツ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>サクセイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>10.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・画面表示時間変数が 1以上 の場合、フィールド描画処理を実行する（）</t>
-    <rPh sb="1" eb="3">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>イジョウ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ビョウガ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ジッコウ</t>
-    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1099,6 +844,394 @@
   </si>
   <si>
     <t>TM</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・アイテムを使用中の場合、アイテム使用時間を -1 する</t>
+    <rPh sb="6" eb="9">
+      <t>シヨウチュウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・タイトル、キー案内の文言を表示（03_DRAW.&lt;文字の描画&gt;）</t>
+    <rPh sb="8" eb="10">
+      <t>アンナイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>モンゴン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ビョウガ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・ゲーム設定を初期化（02_GAME.&lt;ゲームの初期化&gt;）</t>
+    <rPh sb="4" eb="6">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ショキカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・コースフィールド（迷路）の配列を作成（04_FIELD.&lt;フィールド作成&gt;）</t>
+    <rPh sb="10" eb="12">
+      <t>メイロ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ハイレツ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・コースごとのゲーム設定処理を実行（02_GAME.&lt;ゲームの初期配置／初期設定&gt;）</t>
+    <rPh sb="10" eb="12">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・入力された方向キーによってプレイヤーを動かす（05_PLAYER.&lt;プレイヤー操作&gt;）</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ホウコウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ウゴ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・フィールド描画処理を実行する（03_DRAW.&lt;フィールドの描画&gt;）</t>
+    <rPh sb="6" eb="8">
+      <t>ビョウガ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・アイテム使用のチェックを実行する（06_ITEM.&lt;アイテム使用&gt;）</t>
+    <rPh sb="5" eb="7">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・各種オブジェクトのヒット時の処理を実行する（02_GAME.&lt;オブジェクトヒット判定&gt;）</t>
+    <rPh sb="1" eb="3">
+      <t>カクシュ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ハンテイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・ゴール生成判定を実行する（02_GAME.&lt;ゴール生成判定&gt;）</t>
+    <rPh sb="4" eb="8">
+      <t>セイセイハンテイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="26" eb="30">
+      <t>セイセイハンテイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・アイテム生成判定を実行する（06_ITEM.&lt;アイテム生成判定&gt;）</t>
+    <rPh sb="5" eb="9">
+      <t>セイセイハンテイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・アイテム使用中変数が 0 の場合、アイテムの効果を無効化する（06_ITEM.&lt;アイテム無効化&gt;）</t>
+    <rPh sb="5" eb="8">
+      <t>シヨウチュウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="45" eb="48">
+      <t>ムコウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・キー案内の文言を表示（03_DRAW.&lt;文字の描画&gt;）</t>
+    <rPh sb="3" eb="5">
+      <t>アンナイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>モンゴン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・表示中の画面がマニュアル画面以外の場合、画面表示時間を +1 する</t>
+    <rPh sb="13" eb="15">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・画面表示時間が 1 の場合、下記処理を実施</t>
+    <rPh sb="12" eb="14">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="15" eb="19">
+      <t>カキショリ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・ゴールした場合、画面表示時間を初期化する</t>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>ショキカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・表示中の画面がプレイ画面の場合、総プレイ時間を +1 する</t>
+    <rPh sb="1" eb="4">
+      <t>ヒョウジチュウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>★</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>↓ゲーム終了までループ↓</t>
+    <rPh sb="4" eb="6">
+      <t>シュウリョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>↑ゲーム終了までループ↑</t>
+    <rPh sb="4" eb="6">
+      <t>シュウリョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・CONFIGにSEを設定</t>
+    <rPh sb="11" eb="13">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・各種CONFIG情報に初期設定値を格納</t>
+    <rPh sb="1" eb="3">
+      <t>カクシュ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="12" eb="17">
+      <t>ショキセッテイチ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カクノウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・マニュアル（フィールド、エネミー、プレイヤー、操作）を表示</t>
+    <rPh sb="24" eb="26">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>描画の詳細内容は「画面設計書_STB.xlsx（シート：SCR03（マニュアル画面））」を参照</t>
+    <rPh sb="0" eb="2">
+      <t>ビョウガ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>セッケイショ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>描画の詳細内容は「画面設計書_STB.xlsx（シート：SCR04（ゲームクリア画面））」を参照</t>
+    <rPh sb="0" eb="2">
+      <t>ビョウガ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>セッケイショ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>描画の詳細内容は「画面設計書_STB.xlsx（シート：SCR05（ゲームオーバー画面））」を参照</t>
+    <rPh sb="0" eb="2">
+      <t>ビョウガ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>セッケイショ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>描画の詳細内容は「画面設計書_STB.xlsx（シート：SCR01（タイトル画面））」を参照</t>
+    <rPh sb="0" eb="2">
+      <t>ビョウガ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>セッケイショ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>サンショウ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1498,7 +1631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1728,6 +1861,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1737,29 +1894,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1779,15 +1927,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1806,14 +1948,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2299,7 +2435,7 @@
       </c>
       <c r="G15" s="72"/>
       <c r="H15" s="73" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="I15" s="74"/>
       <c r="J15" s="74"/>
@@ -2315,17 +2451,17 @@
       <c r="J16" s="74"/>
       <c r="K16" s="75"/>
       <c r="N16" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="7:16" ht="22.5" customHeight="1">
       <c r="N17" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="7:16" ht="22.5" customHeight="1">
       <c r="N18" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="7:16" ht="22.5" customHeight="1">
@@ -2388,58 +2524,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="84" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
       <c r="P1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="85" t="str">
+      <c r="Q1" s="79" t="str">
         <f>D5</f>
         <v>TM</v>
       </c>
-      <c r="R1" s="85"/>
+      <c r="R1" s="79"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
       <c r="P2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="86">
+      <c r="Q2" s="80">
         <f>B5</f>
         <v>45170</v>
       </c>
-      <c r="R2" s="85"/>
+      <c r="R2" s="79"/>
     </row>
     <row r="3" spans="1:18" ht="22.5" customHeight="1">
       <c r="A3" s="20"/>
@@ -2465,435 +2601,435 @@
       <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87" t="s">
+      <c r="E4" s="81"/>
+      <c r="F4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87" t="s">
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
     </row>
     <row r="5" spans="1:18" ht="22.5" customHeight="1">
       <c r="A5" s="22">
         <v>1</v>
       </c>
-      <c r="B5" s="80">
+      <c r="B5" s="82">
         <v>45170</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81" t="s">
+      <c r="C5" s="82"/>
+      <c r="D5" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="82" t="s">
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="82"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
     </row>
     <row r="6" spans="1:18" ht="22.5" customHeight="1">
       <c r="A6" s="23">
         <v>2</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
     </row>
     <row r="7" spans="1:18" ht="27" customHeight="1">
       <c r="A7" s="23">
         <v>3</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="79"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1">
       <c r="A8" s="23">
         <v>4</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="79"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="79"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1">
       <c r="A9" s="23">
         <v>5</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="79"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="79"/>
-      <c r="Q9" s="79"/>
-      <c r="R9" s="79"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
     </row>
     <row r="10" spans="1:18" ht="27" customHeight="1">
       <c r="A10" s="23">
         <v>6</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1">
       <c r="A11" s="23">
         <v>7</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="79"/>
-      <c r="O11" s="79"/>
-      <c r="P11" s="79"/>
-      <c r="Q11" s="79"/>
-      <c r="R11" s="79"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1">
       <c r="A12" s="23">
         <v>8</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="79"/>
-      <c r="P12" s="79"/>
-      <c r="Q12" s="79"/>
-      <c r="R12" s="79"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
     </row>
     <row r="13" spans="1:18" ht="27" customHeight="1">
       <c r="A13" s="23">
         <v>9</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1">
       <c r="A14" s="23">
         <v>10</v>
       </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="79"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="87"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="87"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="87"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1">
       <c r="A15" s="23">
         <v>11</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
     </row>
     <row r="16" spans="1:18" ht="27" customHeight="1">
       <c r="A16" s="23">
         <v>12</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="87"/>
+      <c r="R16" s="87"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1">
       <c r="A17" s="23">
         <v>13</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="79"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="87"/>
+      <c r="R17" s="87"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1">
       <c r="A18" s="23">
         <v>14</v>
       </c>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="79"/>
-      <c r="R18" s="79"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="87"/>
     </row>
     <row r="19" spans="1:18" ht="27" customHeight="1">
       <c r="A19" s="23">
         <v>15</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="87"/>
+      <c r="R19" s="87"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1">
       <c r="A20" s="23">
         <v>16</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="87"/>
+      <c r="R20" s="87"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1">
       <c r="A21" s="23">
         <v>17</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="87"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="87"/>
     </row>
     <row r="22" spans="1:18" ht="27" customHeight="1">
       <c r="A22" s="23">
         <v>18</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="79"/>
-      <c r="N22" s="79"/>
-      <c r="O22" s="79"/>
-      <c r="P22" s="79"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="79"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="87"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="87"/>
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1"/>
     <row r="24" spans="1:18" ht="27" customHeight="1"/>
@@ -2904,6 +3040,78 @@
     <row r="29" spans="1:18" ht="27" customHeight="1"/>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:R22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:R20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:R17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:R18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:R15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:R16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:R13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:R14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:R11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:R12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:R9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:R10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:R8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:R6"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D1:O2"/>
     <mergeCell ref="Q1:R1"/>
@@ -2912,78 +3120,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:R4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:R6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:R8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:R9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:R10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:R11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:R12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:R13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:R14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:R15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:R16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:R17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:R18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:R20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:R22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.35433070866141736" footer="0.15748031496062992"/>
@@ -2994,10 +3130,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ94"/>
+  <dimension ref="A1:AJ102"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -3013,112 +3149,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="94" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="100" t="str">
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="103" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="94" t="s">
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="104" t="str">
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="89" t="str">
         <f>更新履歴!D5</f>
         <v>TM</v>
       </c>
-      <c r="AB1" s="104"/>
-      <c r="AC1" s="104"/>
-      <c r="AD1" s="104"/>
-      <c r="AE1" s="104" t="s">
+      <c r="AB1" s="89"/>
+      <c r="AC1" s="89"/>
+      <c r="AD1" s="89"/>
+      <c r="AE1" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" s="104"/>
-      <c r="AG1" s="103" t="str">
+      <c r="AF1" s="89"/>
+      <c r="AG1" s="88" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
         <v>TM</v>
       </c>
-      <c r="AH1" s="104"/>
-      <c r="AI1" s="104"/>
-      <c r="AJ1" s="104"/>
+      <c r="AH1" s="89"/>
+      <c r="AI1" s="89"/>
+      <c r="AJ1" s="89"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="97" t="str">
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="100" t="str">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>01_MAIN</v>
       </c>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="99"/>
-      <c r="Y2" s="94" t="s">
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="102"/>
+      <c r="Y2" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="96"/>
-      <c r="AA2" s="105">
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="90">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="105"/>
-      <c r="AC2" s="105"/>
-      <c r="AD2" s="105"/>
-      <c r="AE2" s="104" t="s">
+      <c r="AB2" s="90"/>
+      <c r="AC2" s="90"/>
+      <c r="AD2" s="90"/>
+      <c r="AE2" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="105">
+      <c r="AF2" s="89"/>
+      <c r="AG2" s="90">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="105"/>
-      <c r="AI2" s="105"/>
-      <c r="AJ2" s="105"/>
+      <c r="AH2" s="90"/>
+      <c r="AI2" s="90"/>
+      <c r="AJ2" s="90"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
       <c r="A3" s="35"/>
@@ -3544,7 +3680,7 @@
     </row>
     <row r="16" spans="1:36" ht="15" customHeight="1">
       <c r="A16" s="43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
@@ -3661,7 +3797,9 @@
     </row>
     <row r="22" spans="1:36" ht="15" customHeight="1">
       <c r="A22" s="56"/>
-      <c r="B22" s="17"/>
+      <c r="B22" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="G22" s="17"/>
       <c r="AC22" s="27"/>
       <c r="AD22" s="26"/>
@@ -3673,12 +3811,8 @@
       <c r="AJ22" s="27"/>
     </row>
     <row r="23" spans="1:36" ht="15" customHeight="1">
-      <c r="A23" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="A23" s="56"/>
+      <c r="B23" s="17"/>
       <c r="G23" s="17"/>
       <c r="AC23" s="27"/>
       <c r="AD23" s="26"/>
@@ -3690,9 +3824,11 @@
       <c r="AJ23" s="27"/>
     </row>
     <row r="24" spans="1:36" ht="15" customHeight="1">
-      <c r="A24" s="56"/>
+      <c r="A24" s="56" t="s">
+        <v>118</v>
+      </c>
       <c r="B24" s="17" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="G24" s="17"/>
       <c r="AC24" s="27"/>
@@ -3705,9 +3841,11 @@
       <c r="AJ24" s="27"/>
     </row>
     <row r="25" spans="1:36" ht="15" customHeight="1">
-      <c r="A25" s="56"/>
+      <c r="A25" s="56" t="s">
+        <v>37</v>
+      </c>
       <c r="B25" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G25" s="17"/>
       <c r="AC25" s="27"/>
@@ -3721,7 +3859,9 @@
     </row>
     <row r="26" spans="1:36" ht="15" customHeight="1">
       <c r="A26" s="56"/>
-      <c r="B26" s="17"/>
+      <c r="B26" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="G26" s="17"/>
       <c r="AC26" s="27"/>
       <c r="AD26" s="26"/>
@@ -3733,11 +3873,9 @@
       <c r="AJ26" s="27"/>
     </row>
     <row r="27" spans="1:36" ht="15" customHeight="1">
-      <c r="A27" s="58" t="s">
-        <v>46</v>
-      </c>
+      <c r="A27" s="56"/>
       <c r="B27" s="17" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="G27" s="17"/>
       <c r="AC27" s="27"/>
@@ -3751,9 +3889,7 @@
     </row>
     <row r="28" spans="1:36" ht="15" customHeight="1">
       <c r="A28" s="56"/>
-      <c r="B28" s="17" t="s">
-        <v>49</v>
-      </c>
+      <c r="B28" s="17"/>
       <c r="G28" s="17"/>
       <c r="AC28" s="27"/>
       <c r="AD28" s="26"/>
@@ -3765,9 +3901,11 @@
       <c r="AJ28" s="27"/>
     </row>
     <row r="29" spans="1:36" ht="15" customHeight="1">
-      <c r="A29" s="56"/>
+      <c r="A29" s="58" t="s">
+        <v>44</v>
+      </c>
       <c r="B29" s="17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G29" s="17"/>
       <c r="AC29" s="27"/>
@@ -3781,9 +3919,8 @@
     </row>
     <row r="30" spans="1:36" ht="15" customHeight="1">
       <c r="A30" s="56"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17" t="s">
-        <v>65</v>
+      <c r="B30" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="G30" s="17"/>
       <c r="AC30" s="27"/>
@@ -3797,9 +3934,8 @@
     </row>
     <row r="31" spans="1:36" ht="15" customHeight="1">
       <c r="A31" s="56"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17" t="s">
-        <v>51</v>
+      <c r="B31" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="G31" s="17"/>
       <c r="AC31" s="27"/>
@@ -3814,8 +3950,8 @@
     <row r="32" spans="1:36" ht="15" customHeight="1">
       <c r="A32" s="56"/>
       <c r="B32" s="17"/>
-      <c r="D32" s="17" t="s">
-        <v>52</v>
+      <c r="C32" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="G32" s="17"/>
       <c r="AC32" s="27"/>
@@ -3830,6 +3966,9 @@
     <row r="33" spans="1:36" ht="15" customHeight="1">
       <c r="A33" s="56"/>
       <c r="B33" s="17"/>
+      <c r="C33" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="G33" s="17"/>
       <c r="AC33" s="27"/>
       <c r="AD33" s="26"/>
@@ -3841,11 +3980,10 @@
       <c r="AJ33" s="27"/>
     </row>
     <row r="34" spans="1:36" ht="15" customHeight="1">
-      <c r="A34" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>54</v>
+      <c r="A34" s="56"/>
+      <c r="B34" s="17"/>
+      <c r="D34" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="G34" s="17"/>
       <c r="AC34" s="27"/>
@@ -3859,9 +3997,7 @@
     </row>
     <row r="35" spans="1:36" ht="15" customHeight="1">
       <c r="A35" s="56"/>
-      <c r="B35" s="17" t="s">
-        <v>56</v>
-      </c>
+      <c r="B35" s="17"/>
       <c r="G35" s="17"/>
       <c r="AC35" s="27"/>
       <c r="AD35" s="26"/>
@@ -3873,8 +4009,12 @@
       <c r="AJ35" s="27"/>
     </row>
     <row r="36" spans="1:36" ht="15" customHeight="1">
-      <c r="A36" s="56"/>
-      <c r="B36" s="17"/>
+      <c r="A36" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="G36" s="17"/>
       <c r="AC36" s="27"/>
       <c r="AD36" s="26"/>
@@ -3886,11 +4026,9 @@
       <c r="AJ36" s="27"/>
     </row>
     <row r="37" spans="1:36" ht="15" customHeight="1">
-      <c r="A37" s="58" t="s">
-        <v>55</v>
-      </c>
+      <c r="A37" s="56"/>
       <c r="B37" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G37" s="17"/>
       <c r="AC37" s="27"/>
@@ -3904,9 +4042,7 @@
     </row>
     <row r="38" spans="1:36" ht="15" customHeight="1">
       <c r="A38" s="56"/>
-      <c r="B38" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="B38" s="17"/>
       <c r="G38" s="17"/>
       <c r="AC38" s="27"/>
       <c r="AD38" s="26"/>
@@ -3918,14 +4054,12 @@
       <c r="AJ38" s="27"/>
     </row>
     <row r="39" spans="1:36" ht="15" customHeight="1">
-      <c r="A39" s="56"/>
-      <c r="B39" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
+      <c r="A39" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="G39" s="17"/>
       <c r="AC39" s="27"/>
       <c r="AD39" s="26"/>
@@ -3937,9 +4071,11 @@
       <c r="AJ39" s="27"/>
     </row>
     <row r="40" spans="1:36" ht="15" customHeight="1">
-      <c r="A40" s="56"/>
+      <c r="A40" s="106" t="s">
+        <v>124</v>
+      </c>
       <c r="B40" s="17" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="G40" s="17"/>
       <c r="AC40" s="27"/>
@@ -3954,7 +4090,7 @@
     <row r="41" spans="1:36" ht="15" customHeight="1">
       <c r="A41" s="56"/>
       <c r="B41" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G41" s="17"/>
       <c r="AC41" s="27"/>
@@ -3968,10 +4104,13 @@
     </row>
     <row r="42" spans="1:36" ht="15" customHeight="1">
       <c r="A42" s="56"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17" t="s">
-        <v>60</v>
-      </c>
+      <c r="B42" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
       <c r="G42" s="17"/>
       <c r="AC42" s="27"/>
       <c r="AD42" s="26"/>
@@ -3984,13 +4123,9 @@
     </row>
     <row r="43" spans="1:36" ht="15" customHeight="1">
       <c r="A43" s="56"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
+      <c r="B43" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="G43" s="17"/>
       <c r="AC43" s="27"/>
       <c r="AD43" s="26"/>
@@ -4003,9 +4138,8 @@
     </row>
     <row r="44" spans="1:36" ht="15" customHeight="1">
       <c r="A44" s="56"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17" t="s">
-        <v>62</v>
+      <c r="B44" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G44" s="17"/>
       <c r="AC44" s="27"/>
@@ -4020,6 +4154,9 @@
     <row r="45" spans="1:36" ht="15" customHeight="1">
       <c r="A45" s="56"/>
       <c r="B45" s="17"/>
+      <c r="C45" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="G45" s="17"/>
       <c r="AC45" s="27"/>
       <c r="AD45" s="26"/>
@@ -4031,13 +4168,15 @@
       <c r="AJ45" s="27"/>
     </row>
     <row r="46" spans="1:36" ht="15" customHeight="1">
-      <c r="A46" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G46" s="17"/>
+      <c r="A46" s="56"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
       <c r="AC46" s="27"/>
       <c r="AD46" s="26"/>
       <c r="AE46" s="41"/>
@@ -4048,10 +4187,15 @@
       <c r="AJ46" s="27"/>
     </row>
     <row r="47" spans="1:36" ht="15" customHeight="1">
-      <c r="B47" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="17"/>
+      <c r="A47" s="56"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
       <c r="AC47" s="27"/>
       <c r="AD47" s="26"/>
       <c r="AE47" s="41"/>
@@ -4063,10 +4207,14 @@
     </row>
     <row r="48" spans="1:36" ht="15" customHeight="1">
       <c r="A48" s="56"/>
-      <c r="C48" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
       <c r="AC48" s="27"/>
       <c r="AD48" s="26"/>
       <c r="AE48" s="41"/>
@@ -4078,9 +4226,7 @@
     </row>
     <row r="49" spans="1:36" ht="15" customHeight="1">
       <c r="A49" s="56"/>
-      <c r="D49" s="17" t="s">
-        <v>113</v>
-      </c>
+      <c r="B49" s="17"/>
       <c r="G49" s="17"/>
       <c r="AC49" s="27"/>
       <c r="AD49" s="26"/>
@@ -4092,14 +4238,13 @@
       <c r="AJ49" s="27"/>
     </row>
     <row r="50" spans="1:36" ht="15" customHeight="1">
-      <c r="A50" s="56"/>
-      <c r="C50" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
+      <c r="A50" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="17"/>
       <c r="AC50" s="27"/>
       <c r="AD50" s="26"/>
       <c r="AE50" s="41"/>
@@ -4110,14 +4255,10 @@
       <c r="AJ50" s="27"/>
     </row>
     <row r="51" spans="1:36" ht="15" customHeight="1">
-      <c r="A51" s="56"/>
-      <c r="C51" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
+      <c r="B51" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G51" s="17"/>
       <c r="AC51" s="27"/>
       <c r="AD51" s="26"/>
       <c r="AE51" s="41"/>
@@ -4129,14 +4270,10 @@
     </row>
     <row r="52" spans="1:36" ht="15" customHeight="1">
       <c r="A52" s="56"/>
-      <c r="B52" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="61"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
+      <c r="C52" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="17"/>
       <c r="AC52" s="27"/>
       <c r="AD52" s="26"/>
       <c r="AE52" s="41"/>
@@ -4148,14 +4285,10 @@
     </row>
     <row r="53" spans="1:36" ht="15" customHeight="1">
       <c r="A53" s="56"/>
-      <c r="B53" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
+      <c r="D53" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G53" s="17"/>
       <c r="AC53" s="27"/>
       <c r="AD53" s="26"/>
       <c r="AE53" s="41"/>
@@ -4167,14 +4300,14 @@
     </row>
     <row r="54" spans="1:36" ht="15" customHeight="1">
       <c r="A54" s="56"/>
-      <c r="B54" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
+      <c r="C54" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
       <c r="AC54" s="27"/>
       <c r="AD54" s="26"/>
       <c r="AE54" s="41"/>
@@ -4186,14 +4319,13 @@
     </row>
     <row r="55" spans="1:36" ht="15" customHeight="1">
       <c r="A55" s="56"/>
-      <c r="B55" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="61"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="61"/>
-      <c r="F55" s="61"/>
-      <c r="G55" s="61"/>
+      <c r="C55" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
       <c r="AC55" s="27"/>
       <c r="AD55" s="26"/>
       <c r="AE55" s="41"/>
@@ -4205,14 +4337,14 @@
     </row>
     <row r="56" spans="1:36" ht="15" customHeight="1">
       <c r="A56" s="56"/>
-      <c r="B56" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
+      <c r="B56" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
       <c r="AC56" s="27"/>
       <c r="AD56" s="26"/>
       <c r="AE56" s="41"/>
@@ -4224,14 +4356,15 @@
     </row>
     <row r="57" spans="1:36" ht="15" customHeight="1">
       <c r="A57" s="56"/>
-      <c r="B57" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
-      <c r="G57" s="61"/>
+      <c r="B57" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
       <c r="AC57" s="27"/>
       <c r="AD57" s="26"/>
       <c r="AE57" s="41"/>
@@ -4244,7 +4377,7 @@
     <row r="58" spans="1:36" ht="15" customHeight="1">
       <c r="A58" s="56"/>
       <c r="B58" s="61" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C58" s="61"/>
       <c r="D58" s="61"/>
@@ -4262,14 +4395,14 @@
     </row>
     <row r="59" spans="1:36" ht="15" customHeight="1">
       <c r="A59" s="56"/>
-      <c r="B59" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
+      <c r="B59" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
       <c r="AC59" s="27"/>
       <c r="AD59" s="26"/>
       <c r="AE59" s="41"/>
@@ -4281,10 +4414,14 @@
     </row>
     <row r="60" spans="1:36" ht="15" customHeight="1">
       <c r="A60" s="56"/>
-      <c r="B60" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G60" s="17"/>
+      <c r="B60" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
       <c r="AC60" s="27"/>
       <c r="AD60" s="26"/>
       <c r="AE60" s="41"/>
@@ -4296,21 +4433,14 @@
     </row>
     <row r="61" spans="1:36" ht="15" customHeight="1">
       <c r="A61" s="56"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="61" t="s">
-        <v>78</v>
-      </c>
+      <c r="B61" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="61"/>
       <c r="D61" s="61"/>
       <c r="E61" s="61"/>
       <c r="F61" s="61"/>
       <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="61"/>
-      <c r="K61" s="61"/>
-      <c r="L61" s="61"/>
-      <c r="M61" s="61"/>
-      <c r="N61" s="61"/>
       <c r="AC61" s="27"/>
       <c r="AD61" s="26"/>
       <c r="AE61" s="41"/>
@@ -4322,10 +4452,17 @@
     </row>
     <row r="62" spans="1:36" ht="15" customHeight="1">
       <c r="A62" s="56"/>
-      <c r="B62" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G62" s="17"/>
+      <c r="B62" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
       <c r="AC62" s="27"/>
       <c r="AD62" s="26"/>
       <c r="AE62" s="41"/>
@@ -4337,10 +4474,17 @@
     </row>
     <row r="63" spans="1:36" ht="15" customHeight="1">
       <c r="A63" s="56"/>
-      <c r="B63" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G63" s="17"/>
+      <c r="B63" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+      <c r="J63" s="44"/>
       <c r="AC63" s="27"/>
       <c r="AD63" s="26"/>
       <c r="AE63" s="41"/>
@@ -4353,7 +4497,7 @@
     <row r="64" spans="1:36" ht="15" customHeight="1">
       <c r="A64" s="56"/>
       <c r="B64" s="17" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G64" s="17"/>
       <c r="AC64" s="27"/>
@@ -4368,22 +4512,20 @@
     <row r="65" spans="1:36" ht="15" customHeight="1">
       <c r="A65" s="56"/>
       <c r="B65" s="17"/>
-      <c r="C65" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="63"/>
-      <c r="E65" s="63"/>
-      <c r="F65" s="63"/>
-      <c r="G65" s="66"/>
-      <c r="H65" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="I65" s="64"/>
-      <c r="J65" s="64"/>
-      <c r="K65" s="64"/>
-      <c r="L65" s="64"/>
-      <c r="M65" s="64"/>
-      <c r="N65" s="65"/>
+      <c r="C65" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="44"/>
+      <c r="J65" s="44"/>
+      <c r="K65" s="44"/>
+      <c r="L65" s="44"/>
+      <c r="M65" s="44"/>
+      <c r="N65" s="44"/>
       <c r="AC65" s="27"/>
       <c r="AD65" s="26"/>
       <c r="AE65" s="41"/>
@@ -4395,23 +4537,10 @@
     </row>
     <row r="66" spans="1:36" ht="15" customHeight="1">
       <c r="A66" s="56"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="I66" s="68"/>
-      <c r="J66" s="68"/>
-      <c r="K66" s="68"/>
-      <c r="L66" s="68"/>
-      <c r="M66" s="68"/>
-      <c r="N66" s="60"/>
+      <c r="B66" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G66" s="17"/>
       <c r="AC66" s="27"/>
       <c r="AD66" s="26"/>
       <c r="AE66" s="41"/>
@@ -4423,23 +4552,10 @@
     </row>
     <row r="67" spans="1:36" ht="15" customHeight="1">
       <c r="A67" s="56"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="68"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="60"/>
-      <c r="H67" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="I67" s="68"/>
-      <c r="J67" s="68"/>
-      <c r="K67" s="68"/>
-      <c r="L67" s="68"/>
-      <c r="M67" s="68"/>
-      <c r="N67" s="60"/>
+      <c r="B67" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67" s="17"/>
       <c r="AC67" s="27"/>
       <c r="AD67" s="26"/>
       <c r="AE67" s="41"/>
@@ -4451,23 +4567,10 @@
     </row>
     <row r="68" spans="1:36" ht="15" customHeight="1">
       <c r="A68" s="56"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="D68" s="68"/>
-      <c r="E68" s="68"/>
-      <c r="F68" s="68"/>
-      <c r="G68" s="60"/>
-      <c r="H68" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="I68" s="68"/>
-      <c r="J68" s="68"/>
-      <c r="K68" s="68"/>
-      <c r="L68" s="68"/>
-      <c r="M68" s="68"/>
-      <c r="N68" s="60"/>
+      <c r="B68" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" s="17"/>
       <c r="AC68" s="27"/>
       <c r="AD68" s="26"/>
       <c r="AE68" s="41"/>
@@ -4480,22 +4583,22 @@
     <row r="69" spans="1:36" ht="15" customHeight="1">
       <c r="A69" s="56"/>
       <c r="B69" s="17"/>
-      <c r="C69" s="67" t="s">
-        <v>87</v>
-      </c>
-      <c r="D69" s="68"/>
-      <c r="E69" s="68"/>
-      <c r="F69" s="68"/>
-      <c r="G69" s="60"/>
-      <c r="H69" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="I69" s="68"/>
-      <c r="J69" s="68"/>
-      <c r="K69" s="68"/>
-      <c r="L69" s="68"/>
-      <c r="M69" s="68"/>
-      <c r="N69" s="60"/>
+      <c r="C69" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="66"/>
+      <c r="H69" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="I69" s="64"/>
+      <c r="J69" s="64"/>
+      <c r="K69" s="64"/>
+      <c r="L69" s="64"/>
+      <c r="M69" s="64"/>
+      <c r="N69" s="65"/>
       <c r="AC69" s="27"/>
       <c r="AD69" s="26"/>
       <c r="AE69" s="41"/>
@@ -4508,22 +4611,22 @@
     <row r="70" spans="1:36" ht="15" customHeight="1">
       <c r="A70" s="56"/>
       <c r="B70" s="17"/>
-      <c r="C70" s="69">
-        <v>30</v>
-      </c>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
-      <c r="G70" s="31"/>
+      <c r="C70" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="68"/>
+      <c r="E70" s="68"/>
+      <c r="F70" s="68"/>
+      <c r="G70" s="60"/>
       <c r="H70" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="I70" s="30"/>
-      <c r="J70" s="30"/>
-      <c r="K70" s="30"/>
-      <c r="L70" s="30"/>
-      <c r="M70" s="30"/>
-      <c r="N70" s="31"/>
+        <v>69</v>
+      </c>
+      <c r="I70" s="68"/>
+      <c r="J70" s="68"/>
+      <c r="K70" s="68"/>
+      <c r="L70" s="68"/>
+      <c r="M70" s="68"/>
+      <c r="N70" s="60"/>
       <c r="AC70" s="27"/>
       <c r="AD70" s="26"/>
       <c r="AE70" s="41"/>
@@ -4535,10 +4638,23 @@
     </row>
     <row r="71" spans="1:36" ht="15" customHeight="1">
       <c r="A71" s="56"/>
-      <c r="B71" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="I71" s="68"/>
+      <c r="J71" s="68"/>
+      <c r="K71" s="68"/>
+      <c r="L71" s="68"/>
+      <c r="M71" s="68"/>
+      <c r="N71" s="60"/>
       <c r="AC71" s="27"/>
       <c r="AD71" s="26"/>
       <c r="AE71" s="41"/>
@@ -4551,7 +4667,22 @@
     <row r="72" spans="1:36" ht="15" customHeight="1">
       <c r="A72" s="56"/>
       <c r="B72" s="17"/>
-      <c r="G72" s="17"/>
+      <c r="C72" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="68"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="I72" s="68"/>
+      <c r="J72" s="68"/>
+      <c r="K72" s="68"/>
+      <c r="L72" s="68"/>
+      <c r="M72" s="68"/>
+      <c r="N72" s="60"/>
       <c r="AC72" s="27"/>
       <c r="AD72" s="26"/>
       <c r="AE72" s="41"/>
@@ -4562,13 +4693,24 @@
       <c r="AJ72" s="27"/>
     </row>
     <row r="73" spans="1:36" ht="15" customHeight="1">
-      <c r="A73" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G73" s="17"/>
+      <c r="A73" s="56"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="I73" s="68"/>
+      <c r="J73" s="68"/>
+      <c r="K73" s="68"/>
+      <c r="L73" s="68"/>
+      <c r="M73" s="68"/>
+      <c r="N73" s="60"/>
       <c r="AC73" s="27"/>
       <c r="AD73" s="26"/>
       <c r="AE73" s="41"/>
@@ -4579,12 +4721,24 @@
       <c r="AJ73" s="27"/>
     </row>
     <row r="74" spans="1:36" ht="15" customHeight="1">
-      <c r="A74" s="58"/>
-      <c r="B74" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G74" s="44"/>
-      <c r="H74" s="44"/>
+      <c r="A74" s="56"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="69">
+        <v>30</v>
+      </c>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="30"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="I74" s="30"/>
+      <c r="J74" s="30"/>
+      <c r="K74" s="30"/>
+      <c r="L74" s="30"/>
+      <c r="M74" s="30"/>
+      <c r="N74" s="31"/>
       <c r="AC74" s="27"/>
       <c r="AD74" s="26"/>
       <c r="AE74" s="41"/>
@@ -4596,13 +4750,9 @@
     </row>
     <row r="75" spans="1:36" ht="15" customHeight="1">
       <c r="A75" s="56"/>
-      <c r="B75" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="61"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="61"/>
+      <c r="B75" s="17" t="s">
+        <v>116</v>
+      </c>
       <c r="G75" s="17"/>
       <c r="AC75" s="27"/>
       <c r="AD75" s="26"/>
@@ -4615,9 +4765,7 @@
     </row>
     <row r="76" spans="1:36" ht="15" customHeight="1">
       <c r="A76" s="56"/>
-      <c r="B76" s="17" t="s">
-        <v>99</v>
-      </c>
+      <c r="B76" s="17"/>
       <c r="G76" s="17"/>
       <c r="AC76" s="27"/>
       <c r="AD76" s="26"/>
@@ -4629,8 +4777,12 @@
       <c r="AJ76" s="27"/>
     </row>
     <row r="77" spans="1:36" ht="15" customHeight="1">
-      <c r="A77" s="56"/>
-      <c r="B77" s="17"/>
+      <c r="A77" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="G77" s="17"/>
       <c r="AC77" s="27"/>
       <c r="AD77" s="26"/>
@@ -4642,11 +4794,11 @@
       <c r="AJ77" s="27"/>
     </row>
     <row r="78" spans="1:36" ht="15" customHeight="1">
-      <c r="A78" s="58" t="s">
-        <v>100</v>
+      <c r="A78" s="106" t="s">
+        <v>124</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="G78" s="17"/>
       <c r="AC78" s="27"/>
@@ -4659,15 +4811,12 @@
       <c r="AJ78" s="27"/>
     </row>
     <row r="79" spans="1:36" ht="15" customHeight="1">
-      <c r="A79" s="56"/>
-      <c r="B79" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
-      <c r="E79" s="61"/>
-      <c r="F79" s="61"/>
-      <c r="G79" s="17"/>
+      <c r="A79" s="58"/>
+      <c r="B79" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G79" s="44"/>
+      <c r="H79" s="44"/>
       <c r="AC79" s="27"/>
       <c r="AD79" s="26"/>
       <c r="AE79" s="41"/>
@@ -4679,9 +4828,13 @@
     </row>
     <row r="80" spans="1:36" ht="15" customHeight="1">
       <c r="A80" s="56"/>
-      <c r="B80" s="17" t="s">
-        <v>102</v>
-      </c>
+      <c r="B80" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
       <c r="G80" s="17"/>
       <c r="AC80" s="27"/>
       <c r="AD80" s="26"/>
@@ -4695,7 +4848,7 @@
     <row r="81" spans="1:36" ht="15" customHeight="1">
       <c r="A81" s="56"/>
       <c r="B81" s="17" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="G81" s="17"/>
       <c r="AC81" s="27"/>
@@ -4722,10 +4875,10 @@
     </row>
     <row r="83" spans="1:36" ht="15" customHeight="1">
       <c r="A83" s="58" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G83" s="17"/>
       <c r="AC83" s="27"/>
@@ -4738,14 +4891,12 @@
       <c r="AJ83" s="27"/>
     </row>
     <row r="84" spans="1:36" ht="15" customHeight="1">
-      <c r="A84" s="56"/>
-      <c r="B84" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="61"/>
-      <c r="F84" s="61"/>
+      <c r="A84" s="106" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>126</v>
+      </c>
       <c r="G84" s="17"/>
       <c r="AC84" s="27"/>
       <c r="AD84" s="26"/>
@@ -4758,9 +4909,13 @@
     </row>
     <row r="85" spans="1:36" ht="15" customHeight="1">
       <c r="A85" s="56"/>
-      <c r="B85" s="17" t="s">
-        <v>103</v>
-      </c>
+      <c r="B85" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
       <c r="G85" s="17"/>
       <c r="AC85" s="27"/>
       <c r="AD85" s="26"/>
@@ -4773,6 +4928,9 @@
     </row>
     <row r="86" spans="1:36" ht="15" customHeight="1">
       <c r="A86" s="56"/>
+      <c r="B86" s="17" t="s">
+        <v>86</v>
+      </c>
       <c r="G86" s="17"/>
       <c r="AC86" s="27"/>
       <c r="AD86" s="26"/>
@@ -4784,11 +4942,9 @@
       <c r="AJ86" s="27"/>
     </row>
     <row r="87" spans="1:36" ht="15" customHeight="1">
-      <c r="A87" s="58" t="s">
-        <v>107</v>
-      </c>
+      <c r="A87" s="56"/>
       <c r="B87" s="17" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G87" s="17"/>
       <c r="AC87" s="27"/>
@@ -4802,9 +4958,7 @@
     </row>
     <row r="88" spans="1:36" ht="15" customHeight="1">
       <c r="A88" s="56"/>
-      <c r="B88" s="17" t="s">
-        <v>110</v>
-      </c>
+      <c r="B88" s="17"/>
       <c r="G88" s="17"/>
       <c r="AC88" s="27"/>
       <c r="AD88" s="26"/>
@@ -4816,8 +4970,12 @@
       <c r="AJ88" s="27"/>
     </row>
     <row r="89" spans="1:36" ht="15" customHeight="1">
-      <c r="A89" s="56"/>
-      <c r="B89" s="17"/>
+      <c r="A89" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="G89" s="17"/>
       <c r="AC89" s="27"/>
       <c r="AD89" s="26"/>
@@ -4829,8 +4987,12 @@
       <c r="AJ89" s="27"/>
     </row>
     <row r="90" spans="1:36" ht="15" customHeight="1">
-      <c r="A90" s="56"/>
-      <c r="B90" s="17"/>
+      <c r="A90" s="106" t="s">
+        <v>124</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>127</v>
+      </c>
       <c r="G90" s="17"/>
       <c r="AC90" s="27"/>
       <c r="AD90" s="26"/>
@@ -4842,10 +5004,14 @@
       <c r="AJ90" s="27"/>
     </row>
     <row r="91" spans="1:36" ht="15" customHeight="1">
-      <c r="A91" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="B91" s="17"/>
+      <c r="A91" s="56"/>
+      <c r="B91" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
       <c r="G91" s="17"/>
       <c r="AC91" s="27"/>
       <c r="AD91" s="26"/>
@@ -4857,11 +5023,9 @@
       <c r="AJ91" s="27"/>
     </row>
     <row r="92" spans="1:36" ht="15" customHeight="1">
-      <c r="A92" s="58" t="s">
-        <v>36</v>
-      </c>
+      <c r="A92" s="56"/>
       <c r="B92" s="17" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="G92" s="17"/>
       <c r="AC92" s="27"/>
@@ -4875,7 +5039,6 @@
     </row>
     <row r="93" spans="1:36" ht="15" customHeight="1">
       <c r="A93" s="56"/>
-      <c r="B93" s="17"/>
       <c r="G93" s="17"/>
       <c r="AC93" s="27"/>
       <c r="AD93" s="26"/>
@@ -4887,45 +5050,170 @@
       <c r="AJ93" s="27"/>
     </row>
     <row r="94" spans="1:36" ht="15" customHeight="1">
-      <c r="A94" s="57"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="30"/>
-      <c r="I94" s="30"/>
-      <c r="J94" s="30"/>
-      <c r="K94" s="30"/>
-      <c r="L94" s="30"/>
-      <c r="M94" s="30"/>
-      <c r="N94" s="30"/>
-      <c r="O94" s="30"/>
-      <c r="P94" s="30"/>
-      <c r="Q94" s="30"/>
-      <c r="R94" s="30"/>
-      <c r="S94" s="30"/>
-      <c r="T94" s="30"/>
-      <c r="U94" s="30"/>
-      <c r="V94" s="30"/>
-      <c r="W94" s="30"/>
-      <c r="X94" s="30"/>
-      <c r="Y94" s="30"/>
-      <c r="Z94" s="30"/>
-      <c r="AA94" s="30"/>
-      <c r="AB94" s="30"/>
-      <c r="AC94" s="31"/>
-      <c r="AD94" s="28"/>
-      <c r="AE94" s="30"/>
-      <c r="AF94" s="30"/>
-      <c r="AG94" s="30"/>
-      <c r="AH94" s="30"/>
-      <c r="AI94" s="30"/>
-      <c r="AJ94" s="31"/>
+      <c r="A94" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G94" s="17"/>
+      <c r="AC94" s="27"/>
+      <c r="AD94" s="26"/>
+      <c r="AE94" s="41"/>
+      <c r="AF94" s="41"/>
+      <c r="AG94" s="41"/>
+      <c r="AH94" s="41"/>
+      <c r="AI94" s="41"/>
+      <c r="AJ94" s="27"/>
+    </row>
+    <row r="95" spans="1:36" ht="15" customHeight="1">
+      <c r="A95" s="56"/>
+      <c r="B95" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G95" s="17"/>
+      <c r="AC95" s="27"/>
+      <c r="AD95" s="26"/>
+      <c r="AE95" s="41"/>
+      <c r="AF95" s="41"/>
+      <c r="AG95" s="41"/>
+      <c r="AH95" s="41"/>
+      <c r="AI95" s="41"/>
+      <c r="AJ95" s="27"/>
+    </row>
+    <row r="96" spans="1:36" ht="15" customHeight="1">
+      <c r="A96" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G96" s="17"/>
+      <c r="AC96" s="27"/>
+      <c r="AD96" s="26"/>
+      <c r="AE96" s="41"/>
+      <c r="AF96" s="41"/>
+      <c r="AG96" s="41"/>
+      <c r="AH96" s="41"/>
+      <c r="AI96" s="41"/>
+      <c r="AJ96" s="27"/>
+    </row>
+    <row r="97" spans="1:36" ht="15" customHeight="1">
+      <c r="A97" s="56"/>
+      <c r="B97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="AC97" s="27"/>
+      <c r="AD97" s="26"/>
+      <c r="AE97" s="41"/>
+      <c r="AF97" s="41"/>
+      <c r="AG97" s="41"/>
+      <c r="AH97" s="41"/>
+      <c r="AI97" s="41"/>
+      <c r="AJ97" s="27"/>
+    </row>
+    <row r="98" spans="1:36" ht="15" customHeight="1">
+      <c r="A98" s="56"/>
+      <c r="B98" s="17"/>
+      <c r="G98" s="17"/>
+      <c r="AC98" s="27"/>
+      <c r="AD98" s="26"/>
+      <c r="AE98" s="41"/>
+      <c r="AF98" s="41"/>
+      <c r="AG98" s="41"/>
+      <c r="AH98" s="41"/>
+      <c r="AI98" s="41"/>
+      <c r="AJ98" s="27"/>
+    </row>
+    <row r="99" spans="1:36" ht="15" customHeight="1">
+      <c r="A99" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B99" s="17"/>
+      <c r="G99" s="17"/>
+      <c r="AC99" s="27"/>
+      <c r="AD99" s="26"/>
+      <c r="AE99" s="41"/>
+      <c r="AF99" s="41"/>
+      <c r="AG99" s="41"/>
+      <c r="AH99" s="41"/>
+      <c r="AI99" s="41"/>
+      <c r="AJ99" s="27"/>
+    </row>
+    <row r="100" spans="1:36" ht="15" customHeight="1">
+      <c r="A100" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G100" s="17"/>
+      <c r="AC100" s="27"/>
+      <c r="AD100" s="26"/>
+      <c r="AE100" s="41"/>
+      <c r="AF100" s="41"/>
+      <c r="AG100" s="41"/>
+      <c r="AH100" s="41"/>
+      <c r="AI100" s="41"/>
+      <c r="AJ100" s="27"/>
+    </row>
+    <row r="101" spans="1:36" ht="15" customHeight="1">
+      <c r="A101" s="56"/>
+      <c r="B101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="AC101" s="27"/>
+      <c r="AD101" s="26"/>
+      <c r="AE101" s="41"/>
+      <c r="AF101" s="41"/>
+      <c r="AG101" s="41"/>
+      <c r="AH101" s="41"/>
+      <c r="AI101" s="41"/>
+      <c r="AJ101" s="27"/>
+    </row>
+    <row r="102" spans="1:36" ht="15" customHeight="1">
+      <c r="A102" s="57"/>
+      <c r="B102" s="30"/>
+      <c r="C102" s="30"/>
+      <c r="D102" s="30"/>
+      <c r="E102" s="30"/>
+      <c r="F102" s="30"/>
+      <c r="G102" s="29"/>
+      <c r="H102" s="30"/>
+      <c r="I102" s="30"/>
+      <c r="J102" s="30"/>
+      <c r="K102" s="30"/>
+      <c r="L102" s="30"/>
+      <c r="M102" s="30"/>
+      <c r="N102" s="30"/>
+      <c r="O102" s="30"/>
+      <c r="P102" s="30"/>
+      <c r="Q102" s="30"/>
+      <c r="R102" s="30"/>
+      <c r="S102" s="30"/>
+      <c r="T102" s="30"/>
+      <c r="U102" s="30"/>
+      <c r="V102" s="30"/>
+      <c r="W102" s="30"/>
+      <c r="X102" s="30"/>
+      <c r="Y102" s="30"/>
+      <c r="Z102" s="30"/>
+      <c r="AA102" s="30"/>
+      <c r="AB102" s="30"/>
+      <c r="AC102" s="31"/>
+      <c r="AD102" s="28"/>
+      <c r="AE102" s="30"/>
+      <c r="AF102" s="30"/>
+      <c r="AG102" s="30"/>
+      <c r="AH102" s="30"/>
+      <c r="AI102" s="30"/>
+      <c r="AJ102" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I2:X2"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="AG2:AJ2"/>
     <mergeCell ref="AA1:AD1"/>
@@ -4934,11 +5222,6 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I2:X2"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.35433070866141736" footer="0.15748031496062992"/>

</xml_diff>